<commit_message>
implementing inferenceEngine, updating analyzer
</commit_message>
<xml_diff>
--- a/SmartPlannerApp/ExcelFiles/Path to Graduation 2.xlsx
+++ b/SmartPlannerApp/ExcelFiles/Path to Graduation 2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>Path To Graduation</t>
   </si>
@@ -34,6 +34,12 @@
     <t>Summer 2022</t>
   </si>
   <si>
+    <t>POLS 1101</t>
+  </si>
+  <si>
+    <t>KINS 1105</t>
+  </si>
+  <si>
     <t>Fall 2023</t>
   </si>
   <si>
@@ -43,46 +49,136 @@
     <t>Summer 2023</t>
   </si>
   <si>
-    <t>CPSC 1301K</t>
-  </si>
-  <si>
-    <t>CPSC 1302</t>
-  </si>
-  <si>
-    <t>CPSC 2108</t>
-  </si>
-  <si>
-    <t>CYBR 2159</t>
-  </si>
-  <si>
-    <t>CYBR 2160</t>
-  </si>
-  <si>
-    <t>CYBR 3106</t>
-  </si>
-  <si>
-    <t>CYBR 3108</t>
-  </si>
-  <si>
-    <t>CYBR 3115</t>
-  </si>
-  <si>
-    <t>CYBR 3119</t>
-  </si>
-  <si>
-    <t>CPSC 4111</t>
-  </si>
-  <si>
-    <t>CPSC 4115</t>
-  </si>
-  <si>
-    <t>CPSC 6180</t>
-  </si>
-  <si>
-    <t>CPSC 6185</t>
-  </si>
-  <si>
-    <t>CPSC 6985</t>
+    <t>KINS 1106</t>
+  </si>
+  <si>
+    <t>KINS 2105</t>
+  </si>
+  <si>
+    <t>KINS 2135</t>
+  </si>
+  <si>
+    <t>KINS 2271</t>
+  </si>
+  <si>
+    <t>KINS 2272</t>
+  </si>
+  <si>
+    <t>KINS 2345</t>
+  </si>
+  <si>
+    <t>KINS 2379</t>
+  </si>
+  <si>
+    <t>KINS 3105</t>
+  </si>
+  <si>
+    <t>KINS 3107</t>
+  </si>
+  <si>
+    <t>DSCI 3111</t>
+  </si>
+  <si>
+    <t>CPSC 3121</t>
+  </si>
+  <si>
+    <t>KINS 3126</t>
+  </si>
+  <si>
+    <t>Fall 2024</t>
+  </si>
+  <si>
+    <t>Spring 2024</t>
+  </si>
+  <si>
+    <t>Summer 2024</t>
+  </si>
+  <si>
+    <t>KINS 3127</t>
+  </si>
+  <si>
+    <t>CPSC 3165</t>
+  </si>
+  <si>
+    <t>KINS 3165</t>
+  </si>
+  <si>
+    <t>KINS 3218</t>
+  </si>
+  <si>
+    <t>KINS 3235</t>
+  </si>
+  <si>
+    <t>KINS 3255</t>
+  </si>
+  <si>
+    <t>KINS 3256</t>
+  </si>
+  <si>
+    <t>KINS 3257</t>
+  </si>
+  <si>
+    <t>KINS 3258</t>
+  </si>
+  <si>
+    <t>KINS 3316</t>
+  </si>
+  <si>
+    <t>KINS 3365</t>
+  </si>
+  <si>
+    <t>CPSC 3415</t>
+  </si>
+  <si>
+    <t>CYBR 4125</t>
+  </si>
+  <si>
+    <t>CPSC 4135</t>
+  </si>
+  <si>
+    <t>CYBR 4145</t>
+  </si>
+  <si>
+    <t>CPSC 4148</t>
+  </si>
+  <si>
+    <t>CPSC 4155</t>
+  </si>
+  <si>
+    <t>Fall 2025</t>
+  </si>
+  <si>
+    <t>Spring 2025</t>
+  </si>
+  <si>
+    <t>Summer 2025</t>
+  </si>
+  <si>
+    <t>CPSC 4157</t>
+  </si>
+  <si>
+    <t>CPSC 4175</t>
+  </si>
+  <si>
+    <t>CPSC 4176</t>
+  </si>
+  <si>
+    <t>CPSC 4205</t>
+  </si>
+  <si>
+    <t>CYBR 4416</t>
+  </si>
+  <si>
+    <t>CPSC 4555</t>
+  </si>
+  <si>
+    <t>CPSC 4698</t>
+  </si>
+  <si>
+    <t>CPSC 4899</t>
+  </si>
+  <si>
+    <t>CPSC 4000</t>
   </si>
 </sst>
 </file>
@@ -425,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F20"/>
+  <dimension ref="A2:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,19 +564,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -488,44 +584,98 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -553,19 +703,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
@@ -573,37 +723,111 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19">
         <v>3</v>
       </c>
     </row>
@@ -627,6 +851,144 @@
       </c>
       <c r="F20">
         <f>SUM(F13:F19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <f>SUM(B22:B28)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <f>SUM(D22:D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <f>SUM(F22:F28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <f>SUM(B31:B37)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <f>SUM(D31:D37)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <f>SUM(F31:F37)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>